<commit_message>
Ajustes visuais e funcionais
</commit_message>
<xml_diff>
--- a/xml/28747743/relacao_rubricas.xlsx
+++ b/xml/28747743/relacao_rubricas.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\ConversaoMovimento_eSocial\xml\28747743\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C419C553-940D-4EC6-B0E9-63C712FE28C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Relacionado" sheetId="1" r:id="rId1"/>
     <sheet name="Sem result." sheetId="2" r:id="rId2"/>
     <sheet name="Alerta" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="186">
   <si>
     <t>1</t>
   </si>
@@ -243,6 +249,9 @@
     <t>58005</t>
   </si>
   <si>
+    <t>70005</t>
+  </si>
+  <si>
     <t>70201</t>
   </si>
   <si>
@@ -378,6 +387,9 @@
     <t>Desconto de adto. 13º salário</t>
   </si>
   <si>
+    <t>Saldo de salrio resciso</t>
+  </si>
+  <si>
     <t>Indenização artigo 479</t>
   </si>
   <si>
@@ -502,6 +514,9 @@
   </si>
   <si>
     <t>9214</t>
+  </si>
+  <si>
+    <t>6000</t>
   </si>
   <si>
     <t>6104</t>
@@ -582,8 +597,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -673,6 +688,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -719,7 +742,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -751,9 +774,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -785,6 +826,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -960,12 +1019,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" customWidth="1"/>
@@ -974,11 +1035,11 @@
     <col min="5" max="7" width="26.7109375" customWidth="1"/>
     <col min="8" max="8" width="35.7109375" customWidth="1"/>
     <col min="9" max="9" width="17.7109375" customWidth="1"/>
-    <col min="10" max="10" width="104.7109375" customWidth="1"/>
+    <col min="10" max="10" width="104.7109375" style="1" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="80" customHeight="1">
+    <row r="1" spans="1:10" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>50</v>
       </c>
@@ -1010,7 +1071,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1035,11 +1096,11 @@
       <c r="I2" t="s">
         <v>0</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1067,11 +1128,11 @@
       <c r="I3" t="s">
         <v>41</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1099,11 +1160,11 @@
       <c r="I4" t="s">
         <v>42</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1128,11 +1189,11 @@
       <c r="I5" t="s">
         <v>43</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1160,11 +1221,11 @@
       <c r="I6" t="s">
         <v>44</v>
       </c>
-      <c r="J6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="J6" s="1">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1192,11 +1253,11 @@
       <c r="I7" t="s">
         <v>45</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1221,11 +1282,11 @@
       <c r="I8" t="s">
         <v>46</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1250,11 +1311,11 @@
       <c r="I9" t="s">
         <v>47</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1282,11 +1343,11 @@
       <c r="I10" t="s">
         <v>44</v>
       </c>
-      <c r="J10" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="J10" s="1">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1311,11 +1372,11 @@
       <c r="I11" t="s">
         <v>48</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1340,11 +1401,11 @@
       <c r="I12" t="s">
         <v>44</v>
       </c>
-      <c r="J12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
+      <c r="J12" s="1">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1369,7 +1430,7 @@
       <c r="I13" t="s">
         <v>11</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="1" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1379,12 +1440,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" customWidth="1"/>
     <col min="2" max="2" width="43.7109375" customWidth="1"/>
@@ -1393,11 +1456,11 @@
     <col min="5" max="6" width="26.7109375" customWidth="1"/>
     <col min="7" max="7" width="35.7109375" customWidth="1"/>
     <col min="8" max="8" width="30.7109375" customWidth="1"/>
-    <col min="9" max="9" width="66.7109375" customWidth="1"/>
+    <col min="9" max="9" width="66.7109375" style="1" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="50" customHeight="1">
+    <row r="1" spans="1:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>50</v>
       </c>
@@ -1426,18 +1489,18 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C2" t="s">
         <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="E2" t="s">
         <v>32</v>
@@ -1448,22 +1511,22 @@
       <c r="G2" t="s">
         <v>32</v>
       </c>
-      <c r="I2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="I2" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C3" t="s">
         <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="E3" t="s">
         <v>32</v>
@@ -1474,22 +1537,22 @@
       <c r="G3" t="s">
         <v>32</v>
       </c>
-      <c r="I3" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="I3" s="1">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C4" t="s">
         <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E4" t="s">
         <v>33</v>
@@ -1500,22 +1563,22 @@
       <c r="G4" t="s">
         <v>33</v>
       </c>
-      <c r="I4" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="I4" s="1">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>64</v>
       </c>
       <c r="B5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C5" t="s">
         <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E5" t="s">
         <v>32</v>
@@ -1529,74 +1592,74 @@
       <c r="H5" t="s">
         <v>33</v>
       </c>
-      <c r="I5" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="I5" s="1">
+        <v>8909</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>65</v>
       </c>
       <c r="B6" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C6" t="s">
         <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="E6" t="s">
         <v>33</v>
       </c>
       <c r="F6" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="G6" t="s">
         <v>33</v>
       </c>
-      <c r="I6" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="I6" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>66</v>
       </c>
       <c r="B7" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C7" t="s">
         <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="E7" t="s">
         <v>33</v>
       </c>
       <c r="F7" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="G7" t="s">
         <v>33</v>
       </c>
-      <c r="I7" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="I7" s="1">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>67</v>
       </c>
       <c r="B8" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C8" t="s">
         <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="E8" t="s">
         <v>32</v>
@@ -1610,22 +1673,22 @@
       <c r="H8" t="s">
         <v>33</v>
       </c>
-      <c r="I8" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="I8" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>68</v>
       </c>
       <c r="B9" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C9" t="s">
         <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="E9" t="s">
         <v>33</v>
@@ -1634,21 +1697,21 @@
         <v>37</v>
       </c>
       <c r="G9" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="H9" t="s">
         <v>33</v>
       </c>
-      <c r="I9" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="I9" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>69</v>
       </c>
       <c r="B10" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C10" t="s">
         <v>23</v>
@@ -1665,48 +1728,48 @@
       <c r="G10" t="s">
         <v>32</v>
       </c>
-      <c r="I10" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="I10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>70</v>
       </c>
       <c r="B11" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C11" t="s">
         <v>23</v>
       </c>
       <c r="D11" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="E11" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="F11" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="G11" t="s">
-        <v>175</v>
-      </c>
-      <c r="I11" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+        <v>178</v>
+      </c>
+      <c r="I11" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>71</v>
       </c>
       <c r="B12" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C12" t="s">
         <v>23</v>
       </c>
       <c r="D12" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="E12" t="s">
         <v>32</v>
@@ -1717,22 +1780,22 @@
       <c r="G12" t="s">
         <v>32</v>
       </c>
-      <c r="I12" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="I12" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>72</v>
       </c>
       <c r="B13" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C13" t="s">
         <v>24</v>
       </c>
       <c r="D13" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E13" t="s">
         <v>33</v>
@@ -1741,53 +1804,50 @@
         <v>37</v>
       </c>
       <c r="G13" t="s">
-        <v>175</v>
-      </c>
-      <c r="I13" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+        <v>178</v>
+      </c>
+      <c r="I13" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>73</v>
       </c>
       <c r="B14" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C14" t="s">
         <v>23</v>
       </c>
       <c r="D14" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="E14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F14" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G14" t="s">
-        <v>33</v>
-      </c>
-      <c r="H14" t="s">
-        <v>33</v>
-      </c>
-      <c r="I14" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
+        <v>32</v>
+      </c>
+      <c r="I14" s="1">
+        <v>9179</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>74</v>
       </c>
       <c r="B15" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D15" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="E15" t="s">
         <v>33</v>
@@ -1801,48 +1861,51 @@
       <c r="H15" t="s">
         <v>33</v>
       </c>
-      <c r="I15" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="I15" s="1">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>75</v>
       </c>
       <c r="B16" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D16" t="s">
-        <v>25</v>
+        <v>164</v>
       </c>
       <c r="E16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F16" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="G16" t="s">
-        <v>32</v>
-      </c>
-      <c r="I16" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
+        <v>33</v>
+      </c>
+      <c r="H16" t="s">
+        <v>33</v>
+      </c>
+      <c r="I16" s="1">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>76</v>
       </c>
       <c r="B17" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D17" t="s">
-        <v>162</v>
+        <v>25</v>
       </c>
       <c r="E17" t="s">
         <v>32</v>
@@ -1853,51 +1916,51 @@
       <c r="G17" t="s">
         <v>32</v>
       </c>
-      <c r="H17" t="s">
-        <v>33</v>
-      </c>
-      <c r="I17" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="I17" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>77</v>
       </c>
       <c r="B18" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C18" t="s">
         <v>24</v>
       </c>
       <c r="D18" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F18" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G18" t="s">
-        <v>33</v>
-      </c>
-      <c r="I18" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
+        <v>32</v>
+      </c>
+      <c r="H18" t="s">
+        <v>33</v>
+      </c>
+      <c r="I18" s="1">
+        <v>8792</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>78</v>
       </c>
       <c r="B19" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C19" t="s">
         <v>24</v>
       </c>
       <c r="D19" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="E19" t="s">
         <v>33</v>
@@ -1908,167 +1971,164 @@
       <c r="G19" t="s">
         <v>33</v>
       </c>
-      <c r="I19" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
+      <c r="I19" s="1">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>79</v>
       </c>
       <c r="B20" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C20" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D20" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E20" t="s">
         <v>33</v>
       </c>
       <c r="F20" t="s">
-        <v>177</v>
+        <v>37</v>
       </c>
       <c r="G20" t="s">
-        <v>180</v>
-      </c>
-      <c r="H20" t="s">
-        <v>33</v>
-      </c>
-      <c r="I20" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
+        <v>33</v>
+      </c>
+      <c r="I20" s="1">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>80</v>
       </c>
       <c r="B21" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C21" t="s">
         <v>23</v>
       </c>
       <c r="D21" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="E21" t="s">
         <v>33</v>
       </c>
       <c r="F21" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="G21" t="s">
-        <v>33</v>
+        <v>183</v>
       </c>
       <c r="H21" t="s">
         <v>33</v>
       </c>
-      <c r="I21" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
+      <c r="I21" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>81</v>
       </c>
       <c r="B22" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C22" t="s">
         <v>23</v>
       </c>
       <c r="D22" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="E22" t="s">
         <v>33</v>
       </c>
       <c r="F22" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="G22" t="s">
         <v>33</v>
       </c>
-      <c r="I22" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="H22" t="s">
+        <v>33</v>
+      </c>
+      <c r="I22" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>82</v>
       </c>
       <c r="B23" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C23" t="s">
         <v>23</v>
       </c>
       <c r="D23" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="E23" t="s">
         <v>33</v>
       </c>
       <c r="F23" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="G23" t="s">
         <v>33</v>
       </c>
-      <c r="I23" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
+      <c r="I23" s="1">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>83</v>
       </c>
       <c r="B24" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C24" t="s">
         <v>23</v>
       </c>
       <c r="D24" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="E24" t="s">
         <v>33</v>
       </c>
       <c r="F24" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="G24" t="s">
         <v>33</v>
       </c>
-      <c r="H24" t="s">
-        <v>33</v>
-      </c>
-      <c r="I24" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
+      <c r="I24" s="1">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>84</v>
       </c>
       <c r="B25" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C25" t="s">
         <v>23</v>
       </c>
       <c r="D25" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="E25" t="s">
         <v>33</v>
       </c>
       <c r="F25" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="G25" t="s">
         <v>33</v>
@@ -2076,323 +2136,326 @@
       <c r="H25" t="s">
         <v>33</v>
       </c>
-      <c r="I25" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
+      <c r="I25" s="1">
+        <v>8169</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>85</v>
       </c>
       <c r="B26" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D26" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="E26" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F26" t="s">
-        <v>32</v>
+        <v>180</v>
       </c>
       <c r="G26" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H26" t="s">
         <v>33</v>
       </c>
-      <c r="I26" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
+      <c r="I26" s="1">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>86</v>
       </c>
       <c r="B27" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D27" t="s">
         <v>165</v>
       </c>
       <c r="E27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F27" t="s">
-        <v>177</v>
+        <v>32</v>
       </c>
       <c r="G27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H27" t="s">
         <v>33</v>
       </c>
-      <c r="I27" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
+      <c r="I27" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>87</v>
       </c>
       <c r="B28" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C28" t="s">
         <v>23</v>
       </c>
       <c r="D28" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="E28" t="s">
         <v>33</v>
       </c>
       <c r="F28" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="G28" t="s">
         <v>33</v>
       </c>
-      <c r="I28" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
+      <c r="H28" t="s">
+        <v>33</v>
+      </c>
+      <c r="I28" s="1">
+        <v>8126</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>88</v>
       </c>
       <c r="B29" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C29" t="s">
         <v>23</v>
       </c>
       <c r="D29" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="E29" t="s">
         <v>33</v>
       </c>
       <c r="F29" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="G29" t="s">
         <v>33</v>
       </c>
-      <c r="I29" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
+      <c r="I29" s="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>89</v>
       </c>
       <c r="B30" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C30" t="s">
         <v>23</v>
       </c>
       <c r="D30" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E30" t="s">
-        <v>175</v>
+        <v>33</v>
       </c>
       <c r="F30" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="G30" t="s">
-        <v>175</v>
-      </c>
-      <c r="H30" t="s">
-        <v>33</v>
-      </c>
-      <c r="I30" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
+        <v>33</v>
+      </c>
+      <c r="I30" s="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>90</v>
       </c>
       <c r="B31" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C31" t="s">
         <v>23</v>
       </c>
       <c r="D31" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="E31" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="F31" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="G31" t="s">
-        <v>175</v>
-      </c>
-      <c r="I31" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
+        <v>178</v>
+      </c>
+      <c r="H31" t="s">
+        <v>33</v>
+      </c>
+      <c r="I31" s="1">
+        <v>8550</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>91</v>
       </c>
       <c r="B32" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C32" t="s">
         <v>23</v>
       </c>
       <c r="D32" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="E32" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="F32" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="G32" t="s">
-        <v>175</v>
-      </c>
-      <c r="I32" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9">
+        <v>178</v>
+      </c>
+      <c r="I32" s="1">
+        <v>8551</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>92</v>
       </c>
       <c r="B33" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C33" t="s">
         <v>23</v>
       </c>
       <c r="D33" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="E33" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="F33" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="G33" t="s">
-        <v>180</v>
-      </c>
-      <c r="H33" t="s">
-        <v>33</v>
-      </c>
-      <c r="I33" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9">
+        <v>178</v>
+      </c>
+      <c r="I33" s="1">
+        <v>8552</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>93</v>
       </c>
       <c r="B34" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C34" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D34" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="E34" t="s">
-        <v>33</v>
+        <v>178</v>
       </c>
       <c r="F34" t="s">
-        <v>37</v>
+        <v>178</v>
       </c>
       <c r="G34" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="H34" t="s">
         <v>33</v>
       </c>
-      <c r="I34" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9">
+      <c r="I34" s="1">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>94</v>
       </c>
       <c r="B35" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C35" t="s">
         <v>24</v>
       </c>
       <c r="D35" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="E35" t="s">
-        <v>175</v>
+        <v>33</v>
       </c>
       <c r="F35" t="s">
-        <v>175</v>
+        <v>37</v>
       </c>
       <c r="G35" t="s">
-        <v>175</v>
-      </c>
-      <c r="I35" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9">
+        <v>178</v>
+      </c>
+      <c r="H35" t="s">
+        <v>33</v>
+      </c>
+      <c r="I35" s="1">
+        <v>8566</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>95</v>
       </c>
       <c r="B36" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C36" t="s">
         <v>24</v>
       </c>
       <c r="D36" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="E36" t="s">
-        <v>32</v>
+        <v>178</v>
       </c>
       <c r="F36" t="s">
-        <v>32</v>
+        <v>178</v>
       </c>
       <c r="G36" t="s">
-        <v>32</v>
-      </c>
-      <c r="I36" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9">
+        <v>178</v>
+      </c>
+      <c r="I36" s="1">
+        <v>8566</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>96</v>
       </c>
       <c r="B37" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C37" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D37" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E37" t="s">
         <v>32</v>
@@ -2403,54 +2466,51 @@
       <c r="G37" t="s">
         <v>32</v>
       </c>
-      <c r="H37" t="s">
-        <v>33</v>
-      </c>
-      <c r="I37" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9">
+      <c r="I37" s="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>97</v>
       </c>
       <c r="B38" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C38" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D38" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="E38" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F38" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G38" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H38" t="s">
         <v>33</v>
       </c>
-      <c r="I38" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9">
+      <c r="I38" s="1">
+        <v>8870</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>98</v>
       </c>
       <c r="B39" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C39" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D39" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="E39" t="s">
         <v>33</v>
@@ -2461,45 +2521,45 @@
       <c r="G39" t="s">
         <v>33</v>
       </c>
-      <c r="I39" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9">
+      <c r="H39" t="s">
+        <v>33</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>99</v>
       </c>
       <c r="B40" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C40" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D40" t="s">
-        <v>29</v>
+        <v>176</v>
       </c>
       <c r="E40" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G40" t="s">
         <v>33</v>
       </c>
-      <c r="H40" t="s">
-        <v>33</v>
-      </c>
-      <c r="I40" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9">
+      <c r="I40" s="1">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>100</v>
       </c>
       <c r="B41" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C41" t="s">
         <v>24</v>
@@ -2511,21 +2571,24 @@
         <v>34</v>
       </c>
       <c r="F41" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G41" t="s">
         <v>33</v>
       </c>
-      <c r="I41" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9">
+      <c r="H41" t="s">
+        <v>33</v>
+      </c>
+      <c r="I41" s="1">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>101</v>
       </c>
       <c r="B42" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C42" t="s">
         <v>24</v>
@@ -2534,53 +2597,53 @@
         <v>29</v>
       </c>
       <c r="E42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F42" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G42" t="s">
         <v>33</v>
       </c>
-      <c r="H42" t="s">
-        <v>33</v>
-      </c>
-      <c r="I42" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9">
+      <c r="I42" s="1">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>102</v>
       </c>
       <c r="B43" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C43" t="s">
         <v>24</v>
       </c>
       <c r="D43" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E43" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F43" t="s">
-        <v>179</v>
+        <v>40</v>
       </c>
       <c r="G43" t="s">
         <v>33</v>
       </c>
-      <c r="I43" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9">
+      <c r="H43" t="s">
+        <v>33</v>
+      </c>
+      <c r="I43" s="1">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>103</v>
       </c>
       <c r="B44" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C44" t="s">
         <v>24</v>
@@ -2592,21 +2655,21 @@
         <v>33</v>
       </c>
       <c r="F44" t="s">
-        <v>37</v>
+        <v>182</v>
       </c>
       <c r="G44" t="s">
         <v>33</v>
       </c>
-      <c r="I44" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9">
+      <c r="I44" s="1">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>104</v>
       </c>
       <c r="B45" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C45" t="s">
         <v>24</v>
@@ -2618,39 +2681,65 @@
         <v>33</v>
       </c>
       <c r="F45" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G45" t="s">
         <v>33</v>
       </c>
-      <c r="I45" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9">
+      <c r="I45" s="1">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>105</v>
       </c>
       <c r="B46" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C46" t="s">
-        <v>151</v>
+        <v>24</v>
       </c>
       <c r="D46" t="s">
-        <v>174</v>
+        <v>30</v>
       </c>
       <c r="E46" t="s">
         <v>33</v>
       </c>
       <c r="F46" t="s">
+        <v>35</v>
+      </c>
+      <c r="G46" t="s">
+        <v>33</v>
+      </c>
+      <c r="I46" s="1">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>106</v>
+      </c>
+      <c r="B47" t="s">
+        <v>152</v>
+      </c>
+      <c r="C47" t="s">
+        <v>153</v>
+      </c>
+      <c r="D47" t="s">
+        <v>177</v>
+      </c>
+      <c r="E47" t="s">
+        <v>33</v>
+      </c>
+      <c r="F47" t="s">
         <v>37</v>
       </c>
-      <c r="G46" t="s">
-        <v>33</v>
-      </c>
-      <c r="I46" t="s">
-        <v>181</v>
+      <c r="G47" t="s">
+        <v>33</v>
+      </c>
+      <c r="I47" s="1">
+        <v>996</v>
       </c>
     </row>
   </sheetData>
@@ -2659,12 +2748,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" customWidth="1"/>
@@ -2677,7 +2766,7 @@
     <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="110" customHeight="1">
+    <row r="1" spans="1:10" ht="110.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>50</v>
       </c>
@@ -2706,32 +2795,29 @@
         <v>58</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
         <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H2" t="s">
         <v>33</v>
       </c>
       <c r="I2" t="s">
@@ -2741,7 +2827,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2773,26 +2859,29 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
         <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" t="s">
         <v>34</v>
       </c>
-      <c r="F4" t="s">
-        <v>38</v>
-      </c>
       <c r="G4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" t="s">
         <v>33</v>
       </c>
       <c r="I4" t="s">

</xml_diff>